<commit_message>
EL-EN loss finished. Capacitor selection continue.
</commit_message>
<xml_diff>
--- a/EL-EN 2017/loss/loss_table.xlsx
+++ b/EL-EN 2017/loss/loss_table.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Device</t>
   </si>
@@ -199,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +225,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B25"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +905,7 @@
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="10">
+      <c r="D11" s="11">
         <v>60</v>
       </c>
       <c r="E11" s="1">
@@ -937,7 +941,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="10">
+      <c r="D12" s="11">
         <v>70</v>
       </c>
       <c r="E12" s="1">
@@ -973,7 +977,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="10">
+      <c r="D13" s="11">
         <v>80</v>
       </c>
       <c r="E13" s="1">
@@ -1009,7 +1013,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="10">
+      <c r="D14" s="11">
         <v>90</v>
       </c>
       <c r="E14" s="1">
@@ -1045,7 +1049,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="10">
+      <c r="D15" s="11">
         <v>100</v>
       </c>
       <c r="E15" s="1">
@@ -1267,7 +1271,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="10">
+      <c r="D21" s="11">
         <v>60</v>
       </c>
       <c r="E21" s="1">
@@ -1303,7 +1307,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="10">
+      <c r="D22" s="11">
         <v>70</v>
       </c>
       <c r="E22" s="1">
@@ -1339,7 +1343,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="10">
+      <c r="D23" s="11">
         <v>80</v>
       </c>
       <c r="E23" s="1">
@@ -1375,7 +1379,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="10">
+      <c r="D24" s="11">
         <v>90</v>
       </c>
       <c r="E24" s="1">
@@ -1411,7 +1415,7 @@
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="10">
+      <c r="D25" s="11">
         <v>100</v>
       </c>
       <c r="E25" s="1">
@@ -1461,4 +1465,267 @@
     <ignoredError sqref="I2:I5" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12.93</v>
+      </c>
+      <c r="C2" s="1">
+        <v>31.09</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2" si="0">SUM(B2:E2)</f>
+        <v>53.129999999999995</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2" si="1">F2*6</f>
+        <v>318.77999999999997</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H6" si="2">8000/0.9</f>
+        <v>8888.8888888888887</v>
+      </c>
+      <c r="I2" s="9">
+        <f t="shared" ref="I2" si="3">H2/(G2+H2)*100</f>
+        <v>96.537885931316666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.28</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F4" si="4">SUM(B3:E3)*4</f>
+        <v>25.76</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G4" si="5">F3*6</f>
+        <v>154.56</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="2"/>
+        <v>8888.8888888888887</v>
+      </c>
+      <c r="I3" s="9">
+        <f t="shared" ref="I3:I4" si="6">H3/(G3+H3)*100</f>
+        <v>98.29091752605693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.28</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="4"/>
+        <v>29.400000000000002</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="5"/>
+        <v>176.4</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>8888.8888888888887</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" si="6"/>
+        <v>98.054116066657187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.37</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F6" si="7">SUM(B5:E5)*4</f>
+        <v>24.88</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G7" si="8">F5*6</f>
+        <v>149.28</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>8888.8888888888887</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" ref="I5:I6" si="9">H5/(G5+H5)*100</f>
+        <v>98.348338011435942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>100</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.37</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="7"/>
+        <v>31.8</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="8"/>
+        <v>190.8</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>8888.8888888888887</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="9"/>
+        <v>97.898606413337717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>B6*4</f>
+        <v>17.48</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:E7" si="10">C6*4</f>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="10"/>
+        <v>2.8</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="10"/>
+        <v>3.48</v>
+      </c>
+      <c r="F7" s="10">
+        <f>SUM(B7:E7)</f>
+        <v>31.8</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="8"/>
+        <v>190.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>B4*4</f>
+        <v>21.12</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="11">C4*4</f>
+        <v>4.8</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="11"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="11"/>
+        <v>1.24</v>
+      </c>
+      <c r="F8" s="10">
+        <f>SUM(B8:E8)</f>
+        <v>29.400000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>SUM(B8:C8)</f>
+        <v>25.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>